<commit_message>
Adicionando exibição do excel
</commit_message>
<xml_diff>
--- a/dadosMultiMarket.xlsx
+++ b/dadosMultiMarket.xlsx
@@ -8,17 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1513161F-2AE2-4295-9AF3-2F337AE80591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0673A0C7-DF87-4153-A774-D49252FD7854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7290" yWindow="1755" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Marcel" sheetId="2" r:id="rId2"/>
-    <sheet name="Fabio" sheetId="3" r:id="rId3"/>
-    <sheet name="Fabricio" sheetId="4" r:id="rId4"/>
-    <sheet name="Manoel" sheetId="5" r:id="rId5"/>
-    <sheet name="Renato" sheetId="6" r:id="rId6"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Nome </t>
-  </si>
-  <si>
-    <t>Categoria</t>
-  </si>
-  <si>
-    <t>Preco</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>Banana</t>
   </si>
@@ -50,9 +36,6 @@
     <t>Frango</t>
   </si>
   <si>
-    <t>Carnes</t>
-  </si>
-  <si>
     <t>Cenoura</t>
   </si>
   <si>
@@ -60,22 +43,152 @@
   </si>
   <si>
     <t>Batata</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>preco</t>
+  </si>
+  <si>
+    <t>Feijão</t>
+  </si>
+  <si>
+    <t>Arroz</t>
+  </si>
+  <si>
+    <t>Macarrão</t>
+  </si>
+  <si>
+    <t>Grãos</t>
+  </si>
+  <si>
+    <t>Massas</t>
+  </si>
+  <si>
+    <t>Cebola</t>
+  </si>
+  <si>
+    <t>Maçã</t>
+  </si>
+  <si>
+    <t>Uva</t>
+  </si>
+  <si>
+    <t>Pera</t>
+  </si>
+  <si>
+    <t>Kiwi</t>
+  </si>
+  <si>
+    <t>Água Sanitária</t>
+  </si>
+  <si>
+    <t>Alvajante</t>
+  </si>
+  <si>
+    <t>Detergente</t>
+  </si>
+  <si>
+    <t>Limpeza</t>
+  </si>
+  <si>
+    <t>Sabão em Pó</t>
+  </si>
+  <si>
+    <t>Shampoo</t>
+  </si>
+  <si>
+    <t>Condicionador</t>
+  </si>
+  <si>
+    <t>Ketchup</t>
+  </si>
+  <si>
+    <t>Maionese</t>
+  </si>
+  <si>
+    <t>Mostarda</t>
+  </si>
+  <si>
+    <t>Milho de pipoca</t>
+  </si>
+  <si>
+    <t>Açúcar</t>
+  </si>
+  <si>
+    <t>Sal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macarrão Instantâneo </t>
+  </si>
+  <si>
+    <t>Condimento</t>
+  </si>
+  <si>
+    <t>Batata Frita Congelada</t>
+  </si>
+  <si>
+    <t>Congelados</t>
+  </si>
+  <si>
+    <t>Chã de Dentro</t>
+  </si>
+  <si>
+    <t>Coxão Duro</t>
+  </si>
+  <si>
+    <t>Olive Wagyu</t>
+  </si>
+  <si>
+    <t>Picanha</t>
+  </si>
+  <si>
+    <t>Coxão Mole</t>
+  </si>
+  <si>
+    <t>Carne do Sol</t>
+  </si>
+  <si>
+    <t>Placa de ovo</t>
+  </si>
+  <si>
+    <t>Açougue</t>
+  </si>
+  <si>
+    <t>Olivie Wagyu de pobre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Água </t>
+  </si>
+  <si>
+    <t>Refrigerente</t>
+  </si>
+  <si>
+    <t>Cerveja</t>
+  </si>
+  <si>
+    <t>Vinho</t>
+  </si>
+  <si>
+    <t>Bebidas</t>
+  </si>
+  <si>
+    <t>Margarina</t>
+  </si>
+  <si>
+    <t>Manteiga</t>
+  </si>
+  <si>
+    <t>nome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,12 +216,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,34 +501,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>2.5</v>
@@ -424,10 +535,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1">
         <v>8.5</v>
@@ -435,10 +546,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>0.75</v>
@@ -446,155 +557,402 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4.8</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1">
+        <v>18.989999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12.24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1">
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1">
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="1">
+        <v>39.99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="1">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1">
+        <v>999.99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1">
+        <v>16.899999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="1">
+        <v>8.69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="1">
+        <v>33.89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="1">
+        <v>7.09</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="1">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24626AFA-9911-4BF0-A83C-1A2DB6985D39}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E517769-D213-4BD2-A2F6-5A9131118836}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4049A7EE-5D41-4FED-A925-BAC5BA68C08F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED66EBC3-8361-443C-91D9-9B0D57A54BEA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573C9441-965E-474C-91F2-666CC7276EFE}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>